<commit_message>
Update rem product URL
</commit_message>
<xml_diff>
--- a/backend/Wedding Products.xlsx
+++ b/backend/Wedding Products.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="241">
   <si>
     <t>prod_sku</t>
   </si>
@@ -740,9 +740,6 @@
   </si>
   <si>
     <t>rating</t>
-  </si>
-  <si>
-    <t>https://www.dercodiamonds.com/wp-content/uploads/2021/03/12-Y-1-768x768.jpg</t>
   </si>
   <si>
     <t>rating_count</t>
@@ -1161,7 +1158,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1290,7 @@
         <v>237</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -1484,7 +1481,7 @@
         <v>2450</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>236</v>
@@ -1560,7 +1557,7 @@
         <v>3975</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>236</v>
@@ -1690,7 +1687,7 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="5"/>
       <c r="S7" s="12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>236</v>
@@ -1890,7 +1887,7 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="5"/>
       <c r="S10" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>236</v>
@@ -2144,7 +2141,7 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="5"/>
       <c r="S14" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>236</v>
@@ -2206,7 +2203,7 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="5"/>
       <c r="S15" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>236</v>
@@ -2340,7 +2337,7 @@
       </c>
       <c r="R17" s="5"/>
       <c r="S17" s="12" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="T17" s="3" t="s">
         <v>236</v>
@@ -3616,7 +3613,7 @@
         <v>4610</v>
       </c>
       <c r="S36" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T36" s="3" t="s">
         <v>236</v>
@@ -3694,7 +3691,7 @@
         <v>4150</v>
       </c>
       <c r="S37" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T37" s="3" t="s">
         <v>236</v>
@@ -4290,7 +4287,7 @@
       <c r="Q46" s="3"/>
       <c r="R46" s="5"/>
       <c r="S46" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T46" s="3" t="s">
         <v>236</v>
@@ -4354,7 +4351,7 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="5"/>
       <c r="S47" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T47" s="3" t="s">
         <v>236</v>
@@ -4796,7 +4793,7 @@
         <v>3060</v>
       </c>
       <c r="S53" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T53" s="3" t="s">
         <v>236</v>
@@ -4874,7 +4871,7 @@
         <v>3855</v>
       </c>
       <c r="S54" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T54" s="3" t="s">
         <v>236</v>
@@ -5102,7 +5099,7 @@
         <v>7420</v>
       </c>
       <c r="S57" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T57" s="3" t="s">
         <v>236</v>
@@ -5178,7 +5175,7 @@
         <v>7865</v>
       </c>
       <c r="S58" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="T58" s="3" t="s">
         <v>236</v>
@@ -5218,11 +5215,11 @@
     <hyperlink ref="S3" r:id="rId3" display="https://www.dercodiamonds.com/wp-content/uploads/2021/01/09fdd3a8-eb22-4429-adfa-4627fbd24efa-768x768.jpg"/>
     <hyperlink ref="S4" r:id="rId4" display="https://www.dercodiamonds.com/wp-content/uploads/2022/10/749192_WF-768x768.jpg"/>
     <hyperlink ref="S5" r:id="rId5" display="https://www.dercodiamonds.com/wp-content/uploads/2022/10/749192_RF-768x768.jpg"/>
-    <hyperlink ref="S7" r:id="rId6"/>
+    <hyperlink ref="S7" r:id="rId6" display="https://www.dercodiamonds.com/wp-content/uploads/2021/03/12-Y-1-768x768.jpg"/>
     <hyperlink ref="S13" r:id="rId7" display="https://www.dercodiamonds.com/wp-content/uploads/2021/01/09fdd3a8-eb22-4429-adfa-4627fbd24efa-768x768.jpg"/>
     <hyperlink ref="S14" r:id="rId8" display="https://www.dercodiamonds.com/wp-content/uploads/2022/10/749192_WF-768x768.jpg"/>
     <hyperlink ref="S15" r:id="rId9" display="https://www.dercodiamonds.com/wp-content/uploads/2022/10/749192_RF-768x768.jpg"/>
-    <hyperlink ref="S17" r:id="rId10"/>
+    <hyperlink ref="S17" r:id="rId10" display="https://www.dercodiamonds.com/wp-content/uploads/2021/03/12-Y-1-768x768.jpg"/>
     <hyperlink ref="S9" r:id="rId11" display="https://www.dercodiamonds.com/wp-content/uploads/2021/01/09fdd3a8-eb22-4429-adfa-4627fbd24efa-768x768.jpg"/>
     <hyperlink ref="S10" r:id="rId12" display="https://www.dercodiamonds.com/wp-content/uploads/2022/10/749192_WF-768x768.jpg"/>
     <hyperlink ref="S31" r:id="rId13" display="https://www.dercodiamonds.com/wp-content/uploads/2021/01/09fdd3a8-eb22-4429-adfa-4627fbd24efa-768x768.jpg"/>

</xml_diff>